<commit_message>
terminamos todos los tp
</commit_message>
<xml_diff>
--- a/trabajos practicos/office-integracion/tp2/Complemento MEGA.xlsx
+++ b/trabajos practicos/office-integracion/tp2/Complemento MEGA.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\VSCode Projects\microsoftoffice\microsoftoffice\trabajos practicos\office-integracion\tp2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5D95A2-FF3A-4858-BA73-A0065E8B3DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="19200" windowHeight="11460" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSUMOS" sheetId="2" r:id="rId1"/>
@@ -17,7 +23,20 @@
     <definedName name="noticiero" localSheetId="1">PROGRAMACION!$B$17:$B$21</definedName>
     <definedName name="película" localSheetId="1">PROGRAMACION!$B$27:$B$31</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -183,7 +202,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -264,12 +283,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="51"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="53"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -277,18 +290,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="54"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="44"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -304,8 +305,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -341,19 +360,6 @@
       <bottom style="thin">
         <color indexed="9"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="20"/>
-      </left>
-      <right style="thin">
-        <color indexed="20"/>
-      </right>
-      <top style="thin">
-        <color indexed="20"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -397,7 +403,7 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -405,46 +411,49 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="5" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="5" fillId="10" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -464,6 +473,1015 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-MX"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Porcentajes de Duracion</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="35"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-9752-4F89-A689-48F897960DAF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-9752-4F89-A689-48F897960DAF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="25000"/>
+                      <a:lumOff val="75000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.28943678915135607"/>
+                      <c:h val="0.13567658209390493"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-9752-4F89-A689-48F897960DAF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="25000"/>
+                      <a:lumOff val="75000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.36900787401574797"/>
+                      <c:h val="0.12641732283464566"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-9752-4F89-A689-48F897960DAF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(PROGRAMACION!$B$32,PROGRAMACION!$B$33)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Duración Total (hrs.)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Duración de las Películas (hrs.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(PROGRAMACION!$D$32,PROGRAMACION!$D$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>34.96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6199999999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9752-4F89-A689-48F897960DAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -486,7 +1504,7 @@
         <xdr:cNvPr id="4" name="WordArt 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0CF5B604-C8B1-4ED5-8067-AC9CB52ADE96}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CF5B604-C8B1-4ED5-8067-AC9CB52ADE96}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -625,22 +1643,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="WordArt 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{86D521EF-1FB4-4216-8DF6-C890FF64D161}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86D521EF-1FB4-4216-8DF6-C890FF64D161}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -650,8 +1668,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="523875" y="1304925"/>
-          <a:ext cx="3048000" cy="590550"/>
+          <a:off x="66675" y="342900"/>
+          <a:ext cx="3048000" cy="676275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -698,13 +1716,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DADB0B2D-8A1F-A8A9-0459-4C8FA31D5D60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -742,7 +1796,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -814,7 +1868,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -987,11 +2041,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:J41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B8:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,12 +2055,12 @@
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="6" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>42</v>
       </c>
@@ -1025,626 +2079,809 @@
       <c r="G8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="H8" s="20"/>
+      <c r="I8" s="24" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="18">
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
         <v>43525</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>224</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>1025</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="17">
         <v>8</v>
       </c>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="18">
+      <c r="G9" s="4">
+        <f>PRODUCT(E9,F9)</f>
+        <v>8200</v>
+      </c>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="11">
         <v>43529</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>224</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>1025</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>9</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="7" t="s">
+      <c r="G10" s="4">
+        <f t="shared" ref="G10:G39" si="0">PRODUCT(E10,F10)</f>
+        <v>9225</v>
+      </c>
+      <c r="H10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="18">
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
         <v>43525</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>227</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>248</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>7</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="18">
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>1736</v>
+      </c>
+      <c r="H11" s="21"/>
+      <c r="I11" s="22">
+        <f>SUMIF(D9:D39, "Caja de CDs", F9:F39)</f>
+        <v>24</v>
+      </c>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="11">
         <v>43529</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>227</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>248</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>5</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="18">
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>1240</v>
+      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="11">
         <v>43534</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>227</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>248</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>2</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="7" t="s">
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>496</v>
+      </c>
+      <c r="H13" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="18">
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="11">
         <v>43539</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>227</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>248</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>5</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="18">
+      <c r="G14" s="4">
+        <f t="shared" si="0"/>
+        <v>1240</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="22">
+        <f>SUMIF(D9:D39, "Estanterías", F9:F39)</f>
+        <v>23</v>
+      </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="11">
         <v>43544</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>227</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>248</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>5</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="18">
+      <c r="G15" s="4">
+        <f t="shared" si="0"/>
+        <v>1240</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="11">
         <v>43525</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>224</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>700</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>8</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="7" t="s">
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>5600</v>
+      </c>
+      <c r="H16" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="18">
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="11">
         <v>43525</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>221</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>2100</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>6</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="18">
+      <c r="G17" s="4">
+        <f t="shared" si="0"/>
+        <v>12600</v>
+      </c>
+      <c r="H17" s="20"/>
+      <c r="I17" s="22">
+        <f>SUMIF(D9:D39,"CALCULADORA", F9:F39)</f>
+        <v>27</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
         <v>43529</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>221</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>2100</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>7</v>
       </c>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="18">
+      <c r="G18" s="4">
+        <f t="shared" si="0"/>
+        <v>14700</v>
+      </c>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="11">
         <v>43534</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>221</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>2100</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>4</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="7" t="s">
+      <c r="G19" s="4">
+        <f t="shared" si="0"/>
+        <v>8400</v>
+      </c>
+      <c r="H19" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="20" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="18">
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="11">
         <v>43539</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>221</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>2100</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <v>10</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="7"/>
-      <c r="I20" t="s">
+      <c r="G20" s="4">
+        <f t="shared" si="0"/>
+        <v>21000</v>
+      </c>
+      <c r="H20" s="21"/>
+      <c r="I20" s="20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="18">
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="11">
         <v>43525</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>219</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>180</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <v>8</v>
       </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="18">
+      <c r="G21" s="4">
+        <f t="shared" si="0"/>
+        <v>1440</v>
+      </c>
+      <c r="H21" s="21"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="11">
         <v>43525</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>222</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>152</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <v>2</v>
       </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="16"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="18">
+      <c r="G22" s="4">
+        <f t="shared" si="0"/>
+        <v>304</v>
+      </c>
+      <c r="H22" s="21"/>
+      <c r="I22" s="23">
+        <f>I17/F41</f>
+        <v>0.14594594594594595</v>
+      </c>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="11">
         <v>43529</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>222</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>152</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="5">
         <v>6</v>
       </c>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="18">
+      <c r="G23" s="4">
+        <f t="shared" si="0"/>
+        <v>912</v>
+      </c>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="11">
         <v>43534</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>222</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <v>152</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="5">
         <v>1</v>
       </c>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="18">
+      <c r="G24" s="4">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="11">
         <v>43525</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>215</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>13500</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <v>6</v>
       </c>
-      <c r="G25" s="5"/>
-      <c r="I25" s="15"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="18">
+      <c r="G25" s="4">
+        <f t="shared" si="0"/>
+        <v>81000</v>
+      </c>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="11">
         <v>43534</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <v>215</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <v>13500</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <v>3</v>
       </c>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="18">
+      <c r="G26" s="4">
+        <f t="shared" si="0"/>
+        <v>40500</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="11">
         <v>43544</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>215</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="4">
         <v>13500</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <v>6</v>
       </c>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="18">
+      <c r="G27" s="4">
+        <f t="shared" si="0"/>
+        <v>81000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="11">
         <v>43525</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>221</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="4">
         <v>8500</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="5">
         <v>9</v>
       </c>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="18">
+      <c r="G28" s="4">
+        <f t="shared" si="0"/>
+        <v>76500</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="11">
         <v>43534</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>221</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="4">
         <v>8500</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="5">
         <v>9</v>
       </c>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="18">
+      <c r="G29" s="4">
+        <f t="shared" si="0"/>
+        <v>76500</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="11">
         <v>43525</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>225</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="4">
         <v>2000</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="5">
         <v>9</v>
       </c>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="18">
+      <c r="G30" s="4">
+        <f t="shared" si="0"/>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="11">
         <v>43534</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="3">
         <v>216</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="4">
         <v>2000</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="5">
         <v>10</v>
       </c>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="18">
+      <c r="G31" s="4">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="11">
         <v>43544</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>217</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="4">
         <v>2000</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="5">
         <v>4</v>
       </c>
-      <c r="G32" s="5"/>
+      <c r="G32" s="4">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="18">
+      <c r="B33" s="11">
         <v>43525</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>217</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="4">
         <v>45</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="5">
         <v>1</v>
       </c>
-      <c r="G33" s="5"/>
+      <c r="G33" s="4">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="18">
+      <c r="B34" s="11">
         <v>43525</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>221</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="4">
         <v>15269</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="5">
         <v>5</v>
       </c>
-      <c r="G34" s="5"/>
+      <c r="G34" s="4">
+        <f t="shared" si="0"/>
+        <v>76345</v>
+      </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="18">
+      <c r="B35" s="11">
         <v>43525</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>228</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="4">
         <v>150</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="5">
         <v>8</v>
       </c>
-      <c r="G35" s="5"/>
+      <c r="G35" s="4">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="18">
+      <c r="B36" s="11">
         <v>43534</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="3">
         <v>223</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="4">
         <v>150</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="5">
         <v>2</v>
       </c>
-      <c r="G36" s="5"/>
+      <c r="G36" s="4">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="18">
+      <c r="B37" s="11">
         <v>43525</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <v>229</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="4">
         <v>120</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="5">
         <v>4</v>
       </c>
-      <c r="G37" s="5"/>
+      <c r="G37" s="4">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="18">
+      <c r="B38" s="11">
         <v>43525</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="3">
         <v>220</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="4">
         <v>332</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="5">
         <v>10</v>
       </c>
-      <c r="G38" s="5"/>
+      <c r="G38" s="4">
+        <f t="shared" si="0"/>
+        <v>3320</v>
+      </c>
     </row>
     <row r="39" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="18">
+      <c r="B39" s="11">
         <v>43525</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="3">
         <v>230</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="4">
         <v>10245</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="5">
         <v>6</v>
       </c>
-      <c r="G39" s="19"/>
+      <c r="G39" s="4">
+        <f t="shared" si="0"/>
+        <v>61470</v>
+      </c>
     </row>
     <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="26" t="s">
+      <c r="C40" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="20"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="12">
+        <f>SUM(G9:G39)</f>
+        <v>633145</v>
+      </c>
     </row>
     <row r="41" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="21"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="18">
+        <f>SUM(F9:F39)</f>
+        <v>185</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1658,11 +2895,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:F37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B5:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,335 +2911,432 @@
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F6" s="3" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E6" s="20"/>
+      <c r="F6" s="24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>35</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="8">
         <v>1.66</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" s="20"/>
+      <c r="F8" s="20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="8">
         <v>29</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="8">
         <v>2</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>35</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="8">
         <v>0.76</v>
       </c>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="E10" s="20"/>
+      <c r="F10" s="25">
+        <f>COUNTIF(B8:B31, "noticiero")</f>
+        <v>5</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
         <v>11</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="8">
         <v>1.84</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
         <v>4</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="8">
         <v>1.75</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" s="20"/>
+      <c r="F12" s="20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="8">
         <v>8</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="8">
         <v>1.88</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" s="20"/>
+      <c r="F13" s="20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="8">
         <v>2</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="8">
         <v>1.08</v>
       </c>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+      <c r="E14" s="20"/>
+      <c r="F14" s="25">
+        <f>SUMIF(B8:B31,"novela",D8:D31)</f>
+        <v>7.88</v>
+      </c>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="8">
         <v>8</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="8">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="8">
         <v>2</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="8">
         <v>0.52</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E16" s="20"/>
+      <c r="F16" s="20" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="8">
         <v>2</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="8">
         <v>1.22</v>
       </c>
-      <c r="F17" t="s">
+      <c r="E17" s="20"/>
+      <c r="F17" s="20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="8">
         <v>15</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="8">
         <v>1.37</v>
       </c>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+      <c r="E18" s="20"/>
+      <c r="F18" s="26">
+        <f>D33/D32</f>
+        <v>0.18935926773455375</v>
+      </c>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="8">
         <v>14</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="8">
         <v>1.92</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="8">
         <v>40</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="8">
         <v>1.77</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="8">
         <v>11</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="8">
         <v>0.99</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="8">
         <v>2</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="8">
         <v>1.71</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="8">
         <v>15</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="8">
         <v>1.39</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="8">
         <v>15</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="8">
         <v>1.81</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="8">
         <v>2</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="8">
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="8">
         <v>6</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="8">
         <v>1.88</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="8">
         <v>19</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="8">
         <v>0.64</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="8">
         <v>20</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="8">
         <v>0.66</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="8">
         <v>32</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="8">
         <v>1.96</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="8">
         <v>31</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="8">
         <v>1.8</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="11" t="s">
+    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="8">
         <v>32</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="8">
         <v>1.56</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="24" t="s">
+    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="22"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="19">
+        <f>SUM(D8:D31)</f>
+        <v>34.96</v>
+      </c>
     </row>
     <row r="33" spans="2:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="21"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="13">
+        <f>SUMIF(B8:B31,"película",D8:D31)</f>
+        <v>6.6199999999999992</v>
+      </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="25"/>
+      <c r="D34" s="16"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="14"/>
+      <c r="D35" s="9"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="14"/>
+      <c r="D36" s="9"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="14"/>
+      <c r="D37" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>